<commit_message>
tentando transferir a base de dados
</commit_message>
<xml_diff>
--- a/Coleta.WebAspNet/BaseDadosExcel/Base de Dados.xlsx
+++ b/Coleta.WebAspNet/BaseDadosExcel/Base de Dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCASFERNANDODEASSIS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCASFERNANDODEASSIS\Desktop\ProjetoColetaDados\Coleta.WebAspNet\BaseDadosExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -665,7 +665,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -1248,7 +1248,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1368,62 +1368,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="5" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="6" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="7" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1511,6 +1511,60 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E69E86D9-AA03-4A2E-BA12-4A9EDEA260E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11153775" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoForma 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B69F9836-6CE8-4614-8977-4707707A8246}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1848,47 +1902,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P50" sqref="P50"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="103.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="67.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="215.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="19" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1" style="19"/>
+    <col min="5" max="5" bestFit="1" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="38.42578125" customWidth="1"/>
+    <col min="7" max="7" bestFit="1" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" bestFit="1" width="19.85546875" customWidth="1"/>
+    <col min="10" max="11" bestFit="1" width="18.5703125" customWidth="1"/>
+    <col min="12" max="12" bestFit="1" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" bestFit="1" width="22.7109375" customWidth="1"/>
+    <col min="14" max="14" bestFit="1" width="15.42578125" customWidth="1"/>
+    <col min="15" max="15" bestFit="1" width="31.140625" customWidth="1"/>
+    <col min="16" max="16" bestFit="1" width="44.85546875" customWidth="1"/>
+    <col min="17" max="17" bestFit="1" width="8.140625" customWidth="1"/>
+    <col min="18" max="18" bestFit="1" width="46.7109375" customWidth="1"/>
+    <col min="19" max="19" bestFit="1" width="34.140625" customWidth="1"/>
+    <col min="20" max="20" bestFit="1" width="71.85546875" customWidth="1"/>
+    <col min="21" max="21" bestFit="1" width="64.7109375" customWidth="1"/>
+    <col min="22" max="22" bestFit="1" width="8.140625" customWidth="1"/>
+    <col min="23" max="23" bestFit="1" width="103.85546875" customWidth="1"/>
+    <col min="24" max="24" bestFit="1" width="102.85546875" customWidth="1"/>
+    <col min="25" max="25" bestFit="1" width="30.7109375" customWidth="1"/>
+    <col min="26" max="26" bestFit="1" width="36.85546875" customWidth="1"/>
+    <col min="27" max="27" bestFit="1" width="67.28515625" customWidth="1"/>
+    <col min="28" max="28" bestFit="1" width="45.7109375" customWidth="1"/>
+    <col min="29" max="29" bestFit="1" width="21.85546875" customWidth="1"/>
+    <col min="30" max="30" bestFit="1" width="46.28515625" customWidth="1"/>
+    <col min="31" max="31" bestFit="1" width="215.28515625" customWidth="1"/>
     <col min="32" max="37" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1989,7 +2043,7 @@
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="10">
         <v>42970.426369247682</v>
       </c>
@@ -2076,7 +2130,7 @@
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
     </row>
-    <row r="3" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="10">
         <v>42969.587486597222</v>
       </c>
@@ -2163,9 +2217,9 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
     </row>
-    <row r="4" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="10">
-        <v>42969.617220266198</v>
+        <v>42969.6172202662</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>51</v>
@@ -2252,7 +2306,7 @@
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
     </row>
-    <row r="5" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="10">
         <v>42969.617954895832</v>
       </c>
@@ -2341,7 +2395,7 @@
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
     </row>
-    <row r="6" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="10">
         <v>42969.629874849532</v>
       </c>
@@ -2430,9 +2484,9 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
     </row>
-    <row r="7" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="10">
-        <v>42969.631683703701</v>
+        <v>42969.6316837037</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>66</v>
@@ -2517,7 +2571,7 @@
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="10">
         <v>42969.651186886578</v>
       </c>
@@ -2604,7 +2658,7 @@
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
     </row>
-    <row r="9" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="10">
         <v>42969.662592187495</v>
       </c>
@@ -2693,7 +2747,7 @@
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="10">
         <v>42969.67198353009</v>
       </c>
@@ -2780,7 +2834,7 @@
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="10">
         <v>42969.678679351855</v>
       </c>
@@ -2869,7 +2923,7 @@
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="10">
         <v>42969.689067800922</v>
       </c>
@@ -2954,7 +3008,7 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="10">
         <v>42969.707041087968</v>
       </c>
@@ -3045,7 +3099,7 @@
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
     </row>
-    <row r="14" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="10">
         <v>42969.713294456014</v>
       </c>
@@ -3132,7 +3186,7 @@
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
     </row>
-    <row r="15" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="10">
         <v>42969.737505659723</v>
       </c>
@@ -3221,7 +3275,7 @@
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
     </row>
-    <row r="16" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="10">
         <v>42970.347280231479</v>
       </c>
@@ -3308,7 +3362,7 @@
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="10">
         <v>42970.407396828705</v>
       </c>
@@ -3397,7 +3451,7 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="18" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="10">
         <v>42970.413542071758</v>
       </c>
@@ -3486,7 +3540,7 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
     </row>
-    <row r="19" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="10">
         <v>42970.414752303244</v>
       </c>
@@ -3573,7 +3627,7 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
     </row>
-    <row r="20" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="10">
         <v>42970.41915155093</v>
       </c>
@@ -3660,7 +3714,7 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="10">
         <v>42970.421403483793</v>
       </c>
@@ -3751,9 +3805,9 @@
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="10">
-        <v>42970.422652766203</v>
+        <v>42970.4226527662</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>112</v>
@@ -3840,7 +3894,7 @@
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
     </row>
-    <row r="23" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="10">
         <v>42970.424043252315</v>
       </c>
@@ -3927,7 +3981,7 @@
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="10">
         <v>42970.424517245367</v>
       </c>
@@ -4018,7 +4072,7 @@
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
-    <row r="25" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="10">
         <v>42970.427429212963</v>
       </c>
@@ -4107,7 +4161,7 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
     </row>
-    <row r="26" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="10">
         <v>42970.427995324077</v>
       </c>
@@ -4196,7 +4250,7 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="10">
         <v>42970.427996805556</v>
       </c>
@@ -4287,7 +4341,7 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="10">
         <v>42970.430026817128</v>
       </c>
@@ -4376,7 +4430,7 @@
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="10">
         <v>42970.431458379629</v>
       </c>
@@ -4465,7 +4519,7 @@
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
     </row>
-    <row r="30" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="10">
         <v>42970.493705115739</v>
       </c>
@@ -4552,7 +4606,7 @@
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="10">
         <v>42970.519852546291</v>
       </c>
@@ -4637,7 +4691,7 @@
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="10">
         <v>42970.607316030088</v>
       </c>
@@ -4728,7 +4782,7 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="10">
         <v>42971.306588807871</v>
       </c>
@@ -4817,7 +4871,7 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" ht="12.75">
       <c r="A34" s="10">
         <v>42971.344137048611</v>
       </c>
@@ -4906,7 +4960,7 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" ht="12.75">
       <c r="A35" s="10">
         <v>42971.540662245374</v>
       </c>
@@ -4993,9 +5047,9 @@
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" ht="12.75">
       <c r="A36" s="10">
-        <v>42971.609491249998</v>
+        <v>42971.60949125</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>147</v>
@@ -5080,7 +5134,7 @@
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
     </row>
-    <row r="37" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" ht="12.75">
       <c r="A37" s="10">
         <v>42971.650965775465</v>
       </c>
@@ -5169,7 +5223,7 @@
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" ht="12.75">
       <c r="A38" s="10">
         <v>42971.722634907404</v>
       </c>
@@ -5256,7 +5310,7 @@
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" ht="12.75">
       <c r="A39" s="10">
         <v>42971.791659178241</v>
       </c>
@@ -5343,7 +5397,7 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" ht="12.75">
       <c r="A40" s="10">
         <v>42971.819249363427</v>
       </c>
@@ -5432,7 +5486,7 @@
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" ht="12.75">
       <c r="A41" s="10">
         <v>42971.822113298607</v>
       </c>
@@ -5519,7 +5573,7 @@
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
     </row>
-    <row r="42" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" ht="12.75">
       <c r="A42" s="10">
         <v>42971.826541851857</v>
       </c>
@@ -5610,9 +5664,9 @@
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
-    <row r="43" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" ht="12.75">
       <c r="A43" s="10">
-        <v>42971.826674108801</v>
+        <v>42971.8266741088</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>163</v>
@@ -5701,7 +5755,7 @@
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
     </row>
-    <row r="44" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" ht="12.75">
       <c r="A44" s="10">
         <v>42971.832665798611</v>
       </c>
@@ -5788,7 +5842,7 @@
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" ht="12.75">
       <c r="A45" s="10">
         <v>42971.833669884261</v>
       </c>
@@ -5879,7 +5933,7 @@
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
     </row>
-    <row r="46" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" ht="12.75">
       <c r="A46" s="10">
         <v>42971.835356851851</v>
       </c>
@@ -5968,7 +6022,7 @@
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
     </row>
-    <row r="47" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" ht="12.75">
       <c r="A47" s="10">
         <v>42971.839046863424</v>
       </c>
@@ -6051,9 +6105,9 @@
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
     </row>
-    <row r="48" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" ht="12.75">
       <c r="A48" s="10">
-        <v>42971.845600266199</v>
+        <v>42971.8456002662</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>177</v>
@@ -6142,7 +6196,7 @@
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
     </row>
-    <row r="49" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" ht="12.75">
       <c r="A49" s="10">
         <v>42971.850477175925</v>
       </c>
@@ -6231,7 +6285,7 @@
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
     </row>
-    <row r="50" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" ht="12.75">
       <c r="A50" s="15">
         <v>42970.413715277777</v>
       </c>
@@ -6312,7 +6366,7 @@
       <c r="AJ50" s="1"/>
       <c r="AK50" s="1"/>
     </row>
-    <row r="51" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" ht="12.75">
       <c r="A51" s="15">
         <v>42970.414293981485</v>
       </c>
@@ -6401,7 +6455,7 @@
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
     </row>
-    <row r="52" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" ht="12.75">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -6440,7 +6494,7 @@
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
     </row>
-    <row r="53" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" ht="12.75">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -6479,7 +6533,7 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
     </row>
-    <row r="54" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" ht="12.75">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -6518,7 +6572,7 @@
       <c r="AJ54" s="1"/>
       <c r="AK54" s="1"/>
     </row>
-    <row r="55" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" ht="12.75">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -6557,7 +6611,7 @@
       <c r="AJ55" s="1"/>
       <c r="AK55" s="1"/>
     </row>
-    <row r="56" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" ht="12.75">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -6596,7 +6650,7 @@
       <c r="AJ56" s="1"/>
       <c r="AK56" s="1"/>
     </row>
-    <row r="57" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" ht="12.75">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -6635,7 +6689,7 @@
       <c r="AJ57" s="1"/>
       <c r="AK57" s="1"/>
     </row>
-    <row r="58" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" ht="12.75">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -6674,7 +6728,7 @@
       <c r="AJ58" s="1"/>
       <c r="AK58" s="1"/>
     </row>
-    <row r="59" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" ht="12.75">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -6713,7 +6767,7 @@
       <c r="AJ59" s="1"/>
       <c r="AK59" s="1"/>
     </row>
-    <row r="60" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" ht="12.75">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -6752,7 +6806,7 @@
       <c r="AJ60" s="1"/>
       <c r="AK60" s="1"/>
     </row>
-    <row r="61" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" ht="12.75">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -6791,7 +6845,7 @@
       <c r="AJ61" s="1"/>
       <c r="AK61" s="1"/>
     </row>
-    <row r="62" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" ht="12.75">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -6830,7 +6884,7 @@
       <c r="AJ62" s="1"/>
       <c r="AK62" s="1"/>
     </row>
-    <row r="63" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" ht="12.75">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -6869,7 +6923,7 @@
       <c r="AJ63" s="1"/>
       <c r="AK63" s="1"/>
     </row>
-    <row r="64" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" ht="12.75">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -6908,7 +6962,7 @@
       <c r="AJ64" s="1"/>
       <c r="AK64" s="1"/>
     </row>
-    <row r="65" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" ht="12.75">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -6947,7 +7001,7 @@
       <c r="AJ65" s="1"/>
       <c r="AK65" s="1"/>
     </row>
-    <row r="66" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" ht="12.75">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -6986,7 +7040,7 @@
       <c r="AJ66" s="1"/>
       <c r="AK66" s="1"/>
     </row>
-    <row r="67" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" ht="12.75">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -7025,7 +7079,7 @@
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
     </row>
-    <row r="68" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" ht="12.75">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -7064,7 +7118,7 @@
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
     </row>
-    <row r="69" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" ht="12.75">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -7103,7 +7157,7 @@
       <c r="AJ69" s="1"/>
       <c r="AK69" s="1"/>
     </row>
-    <row r="70" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" ht="12.75">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -7142,7 +7196,7 @@
       <c r="AJ70" s="1"/>
       <c r="AK70" s="1"/>
     </row>
-    <row r="71" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" ht="12.75">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -7181,7 +7235,7 @@
       <c r="AJ71" s="1"/>
       <c r="AK71" s="1"/>
     </row>
-    <row r="72" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" ht="12.75">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -7220,7 +7274,7 @@
       <c r="AJ72" s="1"/>
       <c r="AK72" s="1"/>
     </row>
-    <row r="73" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" ht="12.75">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -7259,7 +7313,7 @@
       <c r="AJ73" s="1"/>
       <c r="AK73" s="1"/>
     </row>
-    <row r="74" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" ht="12.75">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -7298,7 +7352,7 @@
       <c r="AJ74" s="1"/>
       <c r="AK74" s="1"/>
     </row>
-    <row r="75" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" ht="12.75">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -7337,7 +7391,7 @@
       <c r="AJ75" s="1"/>
       <c r="AK75" s="1"/>
     </row>
-    <row r="76" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" ht="12.75">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -7376,7 +7430,7 @@
       <c r="AJ76" s="1"/>
       <c r="AK76" s="1"/>
     </row>
-    <row r="77" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" ht="12.75">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -7415,7 +7469,7 @@
       <c r="AJ77" s="1"/>
       <c r="AK77" s="1"/>
     </row>
-    <row r="78" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" ht="12.75">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -7454,7 +7508,7 @@
       <c r="AJ78" s="1"/>
       <c r="AK78" s="1"/>
     </row>
-    <row r="79" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" ht="12.75">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -7493,7 +7547,7 @@
       <c r="AJ79" s="1"/>
       <c r="AK79" s="1"/>
     </row>
-    <row r="80" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" ht="12.75">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -7532,7 +7586,7 @@
       <c r="AJ80" s="1"/>
       <c r="AK80" s="1"/>
     </row>
-    <row r="81" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" ht="12.75">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -7571,7 +7625,7 @@
       <c r="AJ81" s="1"/>
       <c r="AK81" s="1"/>
     </row>
-    <row r="82" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" ht="12.75">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -7610,7 +7664,7 @@
       <c r="AJ82" s="1"/>
       <c r="AK82" s="1"/>
     </row>
-    <row r="83" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" ht="12.75">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -7649,7 +7703,7 @@
       <c r="AJ83" s="1"/>
       <c r="AK83" s="1"/>
     </row>
-    <row r="84" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" ht="12.75">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -7688,7 +7742,7 @@
       <c r="AJ84" s="1"/>
       <c r="AK84" s="1"/>
     </row>
-    <row r="85" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" ht="12.75">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -7727,7 +7781,7 @@
       <c r="AJ85" s="1"/>
       <c r="AK85" s="1"/>
     </row>
-    <row r="86" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" ht="12.75">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -7766,7 +7820,7 @@
       <c r="AJ86" s="1"/>
       <c r="AK86" s="1"/>
     </row>
-    <row r="87" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" ht="12.75">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -7805,7 +7859,7 @@
       <c r="AJ87" s="1"/>
       <c r="AK87" s="1"/>
     </row>
-    <row r="88" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" ht="12.75">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -7844,7 +7898,7 @@
       <c r="AJ88" s="1"/>
       <c r="AK88" s="1"/>
     </row>
-    <row r="89" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" ht="12.75">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -7883,7 +7937,7 @@
       <c r="AJ89" s="1"/>
       <c r="AK89" s="1"/>
     </row>
-    <row r="90" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" ht="12.75">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -7922,7 +7976,7 @@
       <c r="AJ90" s="1"/>
       <c r="AK90" s="1"/>
     </row>
-    <row r="91" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" ht="12.75">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -7961,7 +8015,7 @@
       <c r="AJ91" s="1"/>
       <c r="AK91" s="1"/>
     </row>
-    <row r="92" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" ht="12.75">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -8000,7 +8054,7 @@
       <c r="AJ92" s="1"/>
       <c r="AK92" s="1"/>
     </row>
-    <row r="93" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" ht="12.75">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -8039,7 +8093,7 @@
       <c r="AJ93" s="1"/>
       <c r="AK93" s="1"/>
     </row>
-    <row r="94" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" ht="12.75">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -8078,7 +8132,7 @@
       <c r="AJ94" s="1"/>
       <c r="AK94" s="1"/>
     </row>
-    <row r="95" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" ht="12.75">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -8117,7 +8171,7 @@
       <c r="AJ95" s="1"/>
       <c r="AK95" s="1"/>
     </row>
-    <row r="96" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" ht="12.75">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -8156,7 +8210,7 @@
       <c r="AJ96" s="1"/>
       <c r="AK96" s="1"/>
     </row>
-    <row r="97" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" ht="12.75">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -8195,7 +8249,7 @@
       <c r="AJ97" s="1"/>
       <c r="AK97" s="1"/>
     </row>
-    <row r="98" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" ht="12.75">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -8234,7 +8288,7 @@
       <c r="AJ98" s="1"/>
       <c r="AK98" s="1"/>
     </row>
-    <row r="99" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" ht="12.75">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -8273,7 +8327,7 @@
       <c r="AJ99" s="1"/>
       <c r="AK99" s="1"/>
     </row>
-    <row r="100" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" ht="12.75">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -8312,7 +8366,7 @@
       <c r="AJ100" s="1"/>
       <c r="AK100" s="1"/>
     </row>
-    <row r="101" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" ht="12.75">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -8351,7 +8405,7 @@
       <c r="AJ101" s="1"/>
       <c r="AK101" s="1"/>
     </row>
-    <row r="102" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" ht="12.75">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -8390,7 +8444,7 @@
       <c r="AJ102" s="1"/>
       <c r="AK102" s="1"/>
     </row>
-    <row r="103" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" ht="12.75">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -8429,7 +8483,7 @@
       <c r="AJ103" s="1"/>
       <c r="AK103" s="1"/>
     </row>
-    <row r="104" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" ht="12.75">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -8468,7 +8522,7 @@
       <c r="AJ104" s="1"/>
       <c r="AK104" s="1"/>
     </row>
-    <row r="105" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" ht="12.75">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -8507,7 +8561,7 @@
       <c r="AJ105" s="1"/>
       <c r="AK105" s="1"/>
     </row>
-    <row r="106" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" ht="12.75">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -8546,7 +8600,7 @@
       <c r="AJ106" s="1"/>
       <c r="AK106" s="1"/>
     </row>
-    <row r="107" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" ht="12.75">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -8585,7 +8639,7 @@
       <c r="AJ107" s="1"/>
       <c r="AK107" s="1"/>
     </row>
-    <row r="108" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" ht="12.75">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -8624,7 +8678,7 @@
       <c r="AJ108" s="1"/>
       <c r="AK108" s="1"/>
     </row>
-    <row r="109" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" ht="12.75">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -8663,7 +8717,7 @@
       <c r="AJ109" s="1"/>
       <c r="AK109" s="1"/>
     </row>
-    <row r="110" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" ht="12.75">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -8702,7 +8756,7 @@
       <c r="AJ110" s="1"/>
       <c r="AK110" s="1"/>
     </row>
-    <row r="111" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" ht="12.75">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -8741,7 +8795,7 @@
       <c r="AJ111" s="1"/>
       <c r="AK111" s="1"/>
     </row>
-    <row r="112" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" ht="12.75">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -8780,7 +8834,7 @@
       <c r="AJ112" s="1"/>
       <c r="AK112" s="1"/>
     </row>
-    <row r="113" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" ht="12.75">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -8819,7 +8873,7 @@
       <c r="AJ113" s="1"/>
       <c r="AK113" s="1"/>
     </row>
-    <row r="114" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" ht="12.75">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -8858,7 +8912,7 @@
       <c r="AJ114" s="1"/>
       <c r="AK114" s="1"/>
     </row>
-    <row r="115" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" ht="12.75">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -8897,7 +8951,7 @@
       <c r="AJ115" s="1"/>
       <c r="AK115" s="1"/>
     </row>
-    <row r="116" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" ht="12.75">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -8936,7 +8990,7 @@
       <c r="AJ116" s="1"/>
       <c r="AK116" s="1"/>
     </row>
-    <row r="117" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" ht="12.75">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -8975,7 +9029,7 @@
       <c r="AJ117" s="1"/>
       <c r="AK117" s="1"/>
     </row>
-    <row r="118" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" ht="12.75">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -9014,7 +9068,7 @@
       <c r="AJ118" s="1"/>
       <c r="AK118" s="1"/>
     </row>
-    <row r="119" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" ht="12.75">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -9053,7 +9107,7 @@
       <c r="AJ119" s="1"/>
       <c r="AK119" s="1"/>
     </row>
-    <row r="120" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" ht="12.75">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -9092,7 +9146,7 @@
       <c r="AJ120" s="1"/>
       <c r="AK120" s="1"/>
     </row>
-    <row r="121" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" ht="12.75">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -9131,7 +9185,7 @@
       <c r="AJ121" s="1"/>
       <c r="AK121" s="1"/>
     </row>
-    <row r="122" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" ht="12.75">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -9170,7 +9224,7 @@
       <c r="AJ122" s="1"/>
       <c r="AK122" s="1"/>
     </row>
-    <row r="123" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" ht="12.75">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -9209,7 +9263,7 @@
       <c r="AJ123" s="1"/>
       <c r="AK123" s="1"/>
     </row>
-    <row r="124" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" ht="12.75">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -9248,7 +9302,7 @@
       <c r="AJ124" s="1"/>
       <c r="AK124" s="1"/>
     </row>
-    <row r="125" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" ht="12.75">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -9287,7 +9341,7 @@
       <c r="AJ125" s="1"/>
       <c r="AK125" s="1"/>
     </row>
-    <row r="126" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" ht="12.75">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -9326,7 +9380,7 @@
       <c r="AJ126" s="1"/>
       <c r="AK126" s="1"/>
     </row>
-    <row r="127" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" ht="12.75">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -9365,7 +9419,7 @@
       <c r="AJ127" s="1"/>
       <c r="AK127" s="1"/>
     </row>
-    <row r="128" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" ht="12.75">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -9404,7 +9458,7 @@
       <c r="AJ128" s="1"/>
       <c r="AK128" s="1"/>
     </row>
-    <row r="129" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" ht="12.75">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -9443,7 +9497,7 @@
       <c r="AJ129" s="1"/>
       <c r="AK129" s="1"/>
     </row>
-    <row r="130" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" ht="12.75">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -9482,7 +9536,7 @@
       <c r="AJ130" s="1"/>
       <c r="AK130" s="1"/>
     </row>
-    <row r="131" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" ht="12.75">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -9521,7 +9575,7 @@
       <c r="AJ131" s="1"/>
       <c r="AK131" s="1"/>
     </row>
-    <row r="132" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" ht="12.75">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -9560,7 +9614,7 @@
       <c r="AJ132" s="1"/>
       <c r="AK132" s="1"/>
     </row>
-    <row r="133" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" ht="12.75">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -9599,7 +9653,7 @@
       <c r="AJ133" s="1"/>
       <c r="AK133" s="1"/>
     </row>
-    <row r="134" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" ht="12.75">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -9638,7 +9692,7 @@
       <c r="AJ134" s="1"/>
       <c r="AK134" s="1"/>
     </row>
-    <row r="135" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" ht="12.75">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -9677,7 +9731,7 @@
       <c r="AJ135" s="1"/>
       <c r="AK135" s="1"/>
     </row>
-    <row r="136" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" ht="12.75">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -9716,7 +9770,7 @@
       <c r="AJ136" s="1"/>
       <c r="AK136" s="1"/>
     </row>
-    <row r="137" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" ht="12.75">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -9755,7 +9809,7 @@
       <c r="AJ137" s="1"/>
       <c r="AK137" s="1"/>
     </row>
-    <row r="138" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" ht="12.75">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -9794,7 +9848,7 @@
       <c r="AJ138" s="1"/>
       <c r="AK138" s="1"/>
     </row>
-    <row r="139" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" ht="12.75">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -9833,7 +9887,7 @@
       <c r="AJ139" s="1"/>
       <c r="AK139" s="1"/>
     </row>
-    <row r="140" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" ht="12.75">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -9872,7 +9926,7 @@
       <c r="AJ140" s="1"/>
       <c r="AK140" s="1"/>
     </row>
-    <row r="141" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" ht="12.75">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -9911,7 +9965,7 @@
       <c r="AJ141" s="1"/>
       <c r="AK141" s="1"/>
     </row>
-    <row r="142" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" ht="12.75">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -9950,7 +10004,7 @@
       <c r="AJ142" s="1"/>
       <c r="AK142" s="1"/>
     </row>
-    <row r="143" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" ht="12.75">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -9989,7 +10043,7 @@
       <c r="AJ143" s="1"/>
       <c r="AK143" s="1"/>
     </row>
-    <row r="144" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" ht="12.75">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -10028,7 +10082,7 @@
       <c r="AJ144" s="1"/>
       <c r="AK144" s="1"/>
     </row>
-    <row r="145" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" ht="12.75">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -10067,7 +10121,7 @@
       <c r="AJ145" s="1"/>
       <c r="AK145" s="1"/>
     </row>
-    <row r="146" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" ht="12.75">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -10106,7 +10160,7 @@
       <c r="AJ146" s="1"/>
       <c r="AK146" s="1"/>
     </row>
-    <row r="147" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" ht="12.75">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -10145,7 +10199,7 @@
       <c r="AJ147" s="1"/>
       <c r="AK147" s="1"/>
     </row>
-    <row r="148" spans="1:37" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" ht="12.75">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -10186,6 +10240,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>